<commit_message>
updated 14000607 moteshakel report had not came by the time
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -18,7 +18,7 @@
     <sheet name="price change" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'data set'!$A$1:$BL$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'data set'!$A$1:$BL$126</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="323">
   <si>
     <t>7فروردین 1400</t>
   </si>
@@ -993,6 +993,12 @@
   </si>
   <si>
     <t>16شهریور1400</t>
+  </si>
+  <si>
+    <t>17شهریور1400</t>
+  </si>
+  <si>
+    <t>روند روزانه بهای سکه و ارز ( چهارشنبه 17 شهریور 1400)</t>
   </si>
 </sst>
 </file>
@@ -4173,11 +4179,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1519335280"/>
-        <c:axId val="1519331472"/>
+        <c:axId val="723862784"/>
+        <c:axId val="723857344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1519335280"/>
+        <c:axId val="723862784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4220,7 +4226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519331472"/>
+        <c:crossAx val="723857344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4228,7 +4234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1519331472"/>
+        <c:axId val="723857344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4279,7 +4285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519335280"/>
+        <c:crossAx val="723862784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7246,8 +7252,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1519321136"/>
-        <c:axId val="1519320592"/>
+        <c:axId val="723850272"/>
+        <c:axId val="723860064"/>
         <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -7399,7 +7405,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>weekly!$A$3</c15:sqref>
@@ -7462,7 +7468,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -7529,7 +7535,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-5F34-4EEC-AA31-125C442C4E54}"/>
                   </c:ext>
@@ -7540,7 +7546,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1519321136"/>
+        <c:axId val="723850272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7583,7 +7589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519320592"/>
+        <c:crossAx val="723860064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7591,7 +7597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1519320592"/>
+        <c:axId val="723860064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7642,7 +7648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519321136"/>
+        <c:crossAx val="723850272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10637,8 +10643,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1519322224"/>
-        <c:axId val="1519335824"/>
+        <c:axId val="723861152"/>
+        <c:axId val="723851360"/>
         <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -10790,7 +10796,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>weekly!$A$3</c15:sqref>
@@ -10853,7 +10859,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -10920,7 +10926,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-CCA6-4C80-96A0-25C22CA7FD99}"/>
                   </c:ext>
@@ -10931,7 +10937,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1519322224"/>
+        <c:axId val="723861152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10974,7 +10980,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519335824"/>
+        <c:crossAx val="723851360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10982,7 +10988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1519335824"/>
+        <c:axId val="723851360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11033,7 +11039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519322224"/>
+        <c:crossAx val="723861152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14018,11 +14024,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1519334736"/>
-        <c:axId val="1519323312"/>
+        <c:axId val="723851904"/>
+        <c:axId val="723859520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1519334736"/>
+        <c:axId val="723851904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14065,7 +14071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519323312"/>
+        <c:crossAx val="723859520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14073,7 +14079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1519323312"/>
+        <c:axId val="723859520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14124,7 +14130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519334736"/>
+        <c:crossAx val="723851904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17109,11 +17115,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1519321680"/>
-        <c:axId val="1519324944"/>
+        <c:axId val="723861696"/>
+        <c:axId val="723862240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1519321680"/>
+        <c:axId val="723861696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17156,7 +17162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519324944"/>
+        <c:crossAx val="723862240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17164,7 +17170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1519324944"/>
+        <c:axId val="723862240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17215,7 +17221,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519321680"/>
+        <c:crossAx val="723861696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20189,11 +20195,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1519332560"/>
-        <c:axId val="1519322768"/>
+        <c:axId val="723852448"/>
+        <c:axId val="723855712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1519332560"/>
+        <c:axId val="723852448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20236,7 +20242,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519322768"/>
+        <c:crossAx val="723855712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20244,7 +20250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1519322768"/>
+        <c:axId val="723855712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20295,7 +20301,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519332560"/>
+        <c:crossAx val="723852448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20421,7 +20427,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="fa-IR" baseline="0"/>
-              <a:t> بازارها( سه‌شنبه 16 شهریور 1400 )</a:t>
+              <a:t> بازارها( چهارشنبه 17 شهریور 1400 )</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -20472,11 +20478,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="62"/>
-          <c:order val="62"/>
+          <c:idx val="63"/>
+          <c:order val="63"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3">
+              <a:schemeClr val="accent4">
                 <a:lumMod val="60000"/>
               </a:schemeClr>
             </a:solidFill>
@@ -20567,21 +20573,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'price change'!$F$64:$I$64</c:f>
+              <c:f>'price change'!$F$65:$I$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.40725657164013329</c:v>
+                  <c:v>1.5117994100294985</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74688796680497926</c:v>
+                  <c:v>0.49423393739703458</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73344741752151099</c:v>
+                  <c:v>9.8365211105892622E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20598,8 +20604,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1519323856"/>
-        <c:axId val="1519324400"/>
+        <c:axId val="723854624"/>
+        <c:axId val="723857888"/>
         <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -20774,7 +20780,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -20847,7 +20853,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-34B6-4AF3-B436-4DC81C3E6FE0}"/>
                   </c:ext>
@@ -20906,7 +20912,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -20979,7 +20985,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-34B6-4AF3-B436-4DC81C3E6FE0}"/>
                   </c:ext>
@@ -21038,7 +21044,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -21111,7 +21117,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-34B6-4AF3-B436-4DC81C3E6FE0}"/>
                   </c:ext>
@@ -21170,7 +21176,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -21243,7 +21249,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-34B6-4AF3-B436-4DC81C3E6FE0}"/>
                   </c:ext>
@@ -21302,7 +21308,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -21375,7 +21381,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-34B6-4AF3-B436-4DC81C3E6FE0}"/>
                   </c:ext>
@@ -21436,7 +21442,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -21509,7 +21515,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-FB1F-4985-99CF-C5CB0831531F}"/>
                   </c:ext>
@@ -21570,7 +21576,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -21643,7 +21649,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-0A64-4372-9B83-0DF3EBC43A06}"/>
                   </c:ext>
@@ -21704,7 +21710,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -21777,7 +21783,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-0A64-4372-9B83-0DF3EBC43A06}"/>
                   </c:ext>
@@ -21838,7 +21844,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -21911,7 +21917,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-0A64-4372-9B83-0DF3EBC43A06}"/>
                   </c:ext>
@@ -21972,7 +21978,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -22045,7 +22051,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-0F7B-461B-B003-FBEFE0DDD362}"/>
                   </c:ext>
@@ -22106,7 +22112,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -22176,7 +22182,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-C173-4A2B-B977-7F984C8BFA84}"/>
                   </c:ext>
@@ -22238,7 +22244,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -22308,7 +22314,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-C173-4A2B-B977-7F984C8BFA84}"/>
                   </c:ext>
@@ -22370,7 +22376,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -22443,7 +22449,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-C173-4A2B-B977-7F984C8BFA84}"/>
                   </c:ext>
@@ -22505,7 +22511,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -22578,7 +22584,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-C173-4A2B-B977-7F984C8BFA84}"/>
                   </c:ext>
@@ -22640,7 +22646,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -22713,7 +22719,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-C173-4A2B-B977-7F984C8BFA84}"/>
                   </c:ext>
@@ -22775,7 +22781,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -22848,7 +22854,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-C173-4A2B-B977-7F984C8BFA84}"/>
                   </c:ext>
@@ -22910,7 +22916,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -22983,7 +22989,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-C173-4A2B-B977-7F984C8BFA84}"/>
                   </c:ext>
@@ -23044,7 +23050,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -23117,7 +23123,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-C173-4A2B-B977-7F984C8BFA84}"/>
                   </c:ext>
@@ -23178,7 +23184,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -23251,7 +23257,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-EE85-428B-812F-1D9F482AFE7A}"/>
                   </c:ext>
@@ -23312,7 +23318,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -23385,7 +23391,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-BA3B-43EA-8A1B-C8AEECBFDEBA}"/>
                   </c:ext>
@@ -23446,7 +23452,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -23519,7 +23525,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-BA3B-43EA-8A1B-C8AEECBFDEBA}"/>
                   </c:ext>
@@ -23580,7 +23586,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -23653,7 +23659,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-BA3B-43EA-8A1B-C8AEECBFDEBA}"/>
                   </c:ext>
@@ -23714,7 +23720,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -23787,7 +23793,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-52ED-4762-B4AC-21DE46265382}"/>
                   </c:ext>
@@ -23849,7 +23855,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -23922,7 +23928,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-474E-47FD-8B08-FE4CFC7C76C1}"/>
                   </c:ext>
@@ -23984,7 +23990,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -24057,7 +24063,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-0148-4577-B119-591850F1711F}"/>
                   </c:ext>
@@ -24119,7 +24125,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -24192,7 +24198,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-0148-4577-B119-591850F1711F}"/>
                   </c:ext>
@@ -24254,7 +24260,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -24327,7 +24333,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-0148-4577-B119-591850F1711F}"/>
                   </c:ext>
@@ -24389,7 +24395,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -24462,7 +24468,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-0148-4577-B119-591850F1711F}"/>
                   </c:ext>
@@ -24524,7 +24530,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -24597,7 +24603,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-0148-4577-B119-591850F1711F}"/>
                   </c:ext>
@@ -24658,7 +24664,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -24731,7 +24737,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-0148-4577-B119-591850F1711F}"/>
                   </c:ext>
@@ -24792,7 +24798,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -24865,7 +24871,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -24926,7 +24932,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -24999,7 +25005,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -25060,7 +25066,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -25133,7 +25139,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -25194,7 +25200,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -25267,7 +25273,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -25328,7 +25334,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -25401,7 +25407,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -25463,7 +25469,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -25536,7 +25542,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -25598,7 +25604,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -25671,7 +25677,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -25733,7 +25739,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -25806,7 +25812,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -25868,7 +25874,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -25941,7 +25947,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-1CEA-4673-9661-2E7333B31E41}"/>
                   </c:ext>
@@ -26003,7 +26009,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -26076,7 +26082,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-190E-4C22-950D-15EBE777B9C3}"/>
                   </c:ext>
@@ -26138,7 +26144,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -26211,7 +26217,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-190E-4C22-950D-15EBE777B9C3}"/>
                   </c:ext>
@@ -26272,7 +26278,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -26345,7 +26351,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-0394-457D-88D1-90642EEC8A74}"/>
                   </c:ext>
@@ -26406,7 +26412,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -26479,7 +26485,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-7D5E-44A9-B1FA-B35A4B4270CE}"/>
                   </c:ext>
@@ -26540,7 +26546,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -26613,7 +26619,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-642D-42BD-9427-3EA0B12E4C25}"/>
                   </c:ext>
@@ -26674,7 +26680,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -26747,7 +26753,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-F251-43F6-8549-1A594C6714C1}"/>
                   </c:ext>
@@ -26808,7 +26814,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -26881,7 +26887,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-F251-43F6-8549-1A594C6714C1}"/>
                   </c:ext>
@@ -26942,7 +26948,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -27015,7 +27021,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-9702-4565-9B43-3EC01CDE7563}"/>
                   </c:ext>
@@ -27077,7 +27083,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -27150,7 +27156,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-2BE7-4DA4-9DB8-45AD71C850B8}"/>
                   </c:ext>
@@ -27212,7 +27218,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -27285,7 +27291,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-2BE7-4DA4-9DB8-45AD71C850B8}"/>
                   </c:ext>
@@ -27347,7 +27353,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -27420,7 +27426,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-2BE7-4DA4-9DB8-45AD71C850B8}"/>
                   </c:ext>
@@ -27482,7 +27488,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -27555,7 +27561,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-2BE7-4DA4-9DB8-45AD71C850B8}"/>
                   </c:ext>
@@ -27617,7 +27623,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -27690,7 +27696,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-76DD-422B-895A-B743B787CE5F}"/>
                   </c:ext>
@@ -27752,7 +27758,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -27825,7 +27831,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-2132-44D5-BA8F-47CBE91EC861}"/>
                   </c:ext>
@@ -27884,7 +27890,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -27957,7 +27963,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-98A7-45F3-8A3F-1BC910C20E36}"/>
                   </c:ext>
@@ -28016,7 +28022,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -28089,7 +28095,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-98A7-45F3-8A3F-1BC910C20E36}"/>
                   </c:ext>
@@ -28148,7 +28154,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -28221,7 +28227,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-98A7-45F3-8A3F-1BC910C20E36}"/>
                   </c:ext>
@@ -28280,7 +28286,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -28353,7 +28359,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-123E-4E08-AA48-A97F75EAA52E}"/>
                   </c:ext>
@@ -28412,7 +28418,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -28485,7 +28491,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-950B-44DB-94DA-03A3DBCD5199}"/>
                   </c:ext>
@@ -28544,7 +28550,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -28673,7 +28679,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -28802,9 +28808,8 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:layout/>
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
                         <c:spPr>
@@ -28878,11 +28883,141 @@
                 </c:val>
               </c15:ser>
             </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="62"/>
+                <c:order val="62"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:layout/>
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'price change'!$F$1:$I$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>دلار</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>سکه</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>طلای 18 عیار</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>شاخص کل بورس</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'price change'!$F$64:$I$64</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>0.40725657164013329</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.74688796680497926</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.73344741752151099</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
           </c:ext>
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1519323856"/>
+        <c:axId val="723854624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28925,7 +29060,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519324400"/>
+        <c:crossAx val="723857888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28933,7 +29068,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1519324400"/>
+        <c:axId val="723857888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28984,7 +29119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519323856"/>
+        <c:crossAx val="723854624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -32886,7 +33021,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32922,7 +33057,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32960,7 +33095,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32998,7 +33133,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33036,7 +33171,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33074,7 +33209,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33117,7 +33252,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33401,10 +33536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM130"/>
+  <dimension ref="A1:BM131"/>
   <sheetViews>
     <sheetView topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W122" sqref="W122"/>
+      <selection activeCell="Y122" sqref="Y122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33491,14 +33626,14 @@
         <v>31</v>
       </c>
       <c r="S1" s="9">
-        <f>L121/G121</f>
+        <f>L122/G122</f>
         <v>2857574.5682051666</v>
       </c>
       <c r="T1" s="9" t="s">
         <v>32</v>
       </c>
       <c r="U1" s="9">
-        <f>M121/K121</f>
+        <f>M122/K122</f>
         <v>28515.368633872931</v>
       </c>
       <c r="V1" s="9" t="s">
@@ -33823,7 +33958,7 @@
         <v>0</v>
       </c>
       <c r="BJ3" t="e">
-        <f t="shared" ref="BJ3:BJ121" si="3">(Y3-O3)/O3</f>
+        <f t="shared" ref="BJ3:BJ122" si="3">(Y3-O3)/O3</f>
         <v>#DIV/0!</v>
       </c>
       <c r="BK3">
@@ -41536,7 +41671,7 @@
         <v>1.6382373845060413E-2</v>
       </c>
       <c r="BK62" s="32">
-        <f>K121/K62</f>
+        <f>K122/K62</f>
         <v>136.05209774089442</v>
       </c>
       <c r="BL62">
@@ -47402,36 +47537,36 @@
       <c r="BG119" s="71"/>
       <c r="BH119" s="71"/>
     </row>
-    <row r="120" spans="1:62" s="58" customFormat="1" ht="21" customHeight="1">
-      <c r="A120" s="55"/>
-      <c r="B120" s="56" t="s">
+    <row r="120" spans="1:62" s="69" customFormat="1" ht="21" customHeight="1">
+      <c r="A120" s="66"/>
+      <c r="B120" s="67" t="s">
         <v>320</v>
       </c>
-      <c r="C120" s="56">
+      <c r="C120" s="67">
         <v>16</v>
       </c>
-      <c r="D120" s="57">
+      <c r="D120" s="68">
         <v>26570</v>
       </c>
-      <c r="E120" s="56">
+      <c r="E120" s="67">
         <v>26360</v>
       </c>
-      <c r="F120" s="56">
+      <c r="F120" s="67">
         <v>26384</v>
       </c>
-      <c r="G120" s="56">
+      <c r="G120" s="67">
         <v>7781600</v>
       </c>
-      <c r="H120" s="56">
+      <c r="H120" s="67">
         <v>31212</v>
       </c>
-      <c r="I120" s="56">
+      <c r="I120" s="67">
         <v>31350</v>
       </c>
-      <c r="J120" s="56">
+      <c r="J120" s="67">
         <v>31111</v>
       </c>
-      <c r="K120" s="56">
+      <c r="K120" s="67">
         <v>1167200</v>
       </c>
       <c r="L120" s="67">
@@ -47442,218 +47577,294 @@
         <f t="shared" si="13"/>
         <v>36312759200</v>
       </c>
-      <c r="N120" s="58">
+      <c r="N120" s="69">
         <v>26623</v>
       </c>
-      <c r="O120" s="58">
+      <c r="O120" s="69">
         <v>31663</v>
       </c>
-      <c r="P120" s="56">
+      <c r="P120" s="67">
         <v>26836</v>
       </c>
-      <c r="Q120" s="58">
+      <c r="Q120" s="69">
         <v>31525</v>
       </c>
-      <c r="R120" s="56"/>
-      <c r="S120" s="56"/>
-      <c r="T120" s="56"/>
-      <c r="U120" s="56"/>
-      <c r="V120" s="58">
+      <c r="R120" s="67"/>
+      <c r="S120" s="67"/>
+      <c r="T120" s="67"/>
+      <c r="U120" s="67"/>
+      <c r="V120" s="69">
         <v>27180</v>
       </c>
-      <c r="X120" s="58">
+      <c r="X120" s="69">
         <v>27120</v>
       </c>
-      <c r="Y120" s="58">
+      <c r="Y120" s="69">
         <v>32297</v>
       </c>
-      <c r="Z120" s="56"/>
-      <c r="AA120" s="56"/>
-      <c r="AB120" s="56"/>
-      <c r="AC120" s="56"/>
-      <c r="AD120" s="56"/>
-      <c r="AE120" s="56"/>
-      <c r="AF120" s="56"/>
-      <c r="AG120" s="56"/>
-      <c r="AH120" s="56"/>
-      <c r="AI120" s="56"/>
-      <c r="AJ120" s="56"/>
-      <c r="AK120" s="56"/>
-      <c r="AL120" s="56"/>
-      <c r="AM120" s="56"/>
-      <c r="AN120" s="56"/>
-      <c r="AO120" s="56"/>
-      <c r="AP120" s="56"/>
-      <c r="AQ120" s="56"/>
-      <c r="AR120" s="56"/>
-      <c r="AS120" s="57"/>
-      <c r="AT120" s="57"/>
-      <c r="AU120" s="57"/>
-      <c r="AV120" s="57"/>
-      <c r="AW120" s="57"/>
-      <c r="AX120" s="57"/>
-      <c r="AY120" s="56"/>
-      <c r="AZ120" s="56"/>
-      <c r="BA120" s="56"/>
-      <c r="BB120" s="56"/>
-      <c r="BC120" s="56"/>
-      <c r="BE120" s="59"/>
-      <c r="BF120" s="59"/>
-      <c r="BG120" s="59"/>
-      <c r="BH120" s="59"/>
-    </row>
-    <row r="121" spans="1:62" ht="18">
-      <c r="A121" s="6"/>
-      <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
-      <c r="D121" s="19"/>
-      <c r="E121" s="7"/>
-      <c r="F121" s="7"/>
-      <c r="G121" s="7">
+      <c r="Z120" s="67"/>
+      <c r="AA120" s="67"/>
+      <c r="AB120" s="67"/>
+      <c r="AC120" s="67"/>
+      <c r="AD120" s="67"/>
+      <c r="AE120" s="67"/>
+      <c r="AF120" s="67"/>
+      <c r="AG120" s="67"/>
+      <c r="AH120" s="67"/>
+      <c r="AI120" s="67"/>
+      <c r="AJ120" s="67"/>
+      <c r="AK120" s="67"/>
+      <c r="AL120" s="67"/>
+      <c r="AM120" s="67"/>
+      <c r="AN120" s="67"/>
+      <c r="AO120" s="67"/>
+      <c r="AP120" s="67"/>
+      <c r="AQ120" s="67"/>
+      <c r="AR120" s="67"/>
+      <c r="AS120" s="68"/>
+      <c r="AT120" s="68"/>
+      <c r="AU120" s="68"/>
+      <c r="AV120" s="68"/>
+      <c r="AW120" s="68"/>
+      <c r="AX120" s="68"/>
+      <c r="AY120" s="67"/>
+      <c r="AZ120" s="67"/>
+      <c r="BA120" s="67"/>
+      <c r="BB120" s="67"/>
+      <c r="BC120" s="67"/>
+      <c r="BE120" s="71"/>
+      <c r="BF120" s="71"/>
+      <c r="BG120" s="71"/>
+      <c r="BH120" s="71"/>
+    </row>
+    <row r="121" spans="1:62" s="58" customFormat="1" ht="21" customHeight="1">
+      <c r="A121" s="55"/>
+      <c r="B121" s="56" t="s">
+        <v>321</v>
+      </c>
+      <c r="C121" s="56">
+        <v>17</v>
+      </c>
+      <c r="D121" s="57">
+        <v>26681</v>
+      </c>
+      <c r="E121" s="56"/>
+      <c r="F121" s="56"/>
+      <c r="G121" s="56"/>
+      <c r="H121" s="56">
+        <v>31234</v>
+      </c>
+      <c r="I121" s="56"/>
+      <c r="J121" s="56"/>
+      <c r="K121" s="56"/>
+      <c r="L121" s="67"/>
+      <c r="M121" s="67"/>
+      <c r="N121" s="58">
+        <v>26852</v>
+      </c>
+      <c r="O121" s="58">
+        <v>31530</v>
+      </c>
+      <c r="P121" s="56">
+        <v>26948</v>
+      </c>
+      <c r="Q121" s="58">
+        <v>31547</v>
+      </c>
+      <c r="R121" s="56"/>
+      <c r="S121" s="56"/>
+      <c r="T121" s="56"/>
+      <c r="U121" s="56"/>
+      <c r="V121" s="58">
+        <v>27570</v>
+      </c>
+      <c r="Z121" s="56"/>
+      <c r="AA121" s="56"/>
+      <c r="AB121" s="56"/>
+      <c r="AC121" s="56"/>
+      <c r="AD121" s="56"/>
+      <c r="AE121" s="56"/>
+      <c r="AF121" s="56"/>
+      <c r="AG121" s="56"/>
+      <c r="AH121" s="56"/>
+      <c r="AI121" s="56"/>
+      <c r="AJ121" s="56"/>
+      <c r="AK121" s="56"/>
+      <c r="AL121" s="56"/>
+      <c r="AM121" s="56"/>
+      <c r="AN121" s="56"/>
+      <c r="AO121" s="56"/>
+      <c r="AP121" s="56"/>
+      <c r="AQ121" s="56"/>
+      <c r="AR121" s="56"/>
+      <c r="AS121" s="57"/>
+      <c r="AT121" s="57"/>
+      <c r="AU121" s="57"/>
+      <c r="AV121" s="57"/>
+      <c r="AW121" s="57"/>
+      <c r="AX121" s="57"/>
+      <c r="AY121" s="56"/>
+      <c r="AZ121" s="56"/>
+      <c r="BA121" s="56"/>
+      <c r="BB121" s="56"/>
+      <c r="BC121" s="56"/>
+      <c r="BE121" s="59"/>
+      <c r="BF121" s="59"/>
+      <c r="BG121" s="59"/>
+      <c r="BH121" s="59"/>
+    </row>
+    <row r="122" spans="1:62" ht="18">
+      <c r="A122" s="6"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="7"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="7"/>
+      <c r="G122" s="7">
         <f>SUM(G2:G119)/118</f>
         <v>5801599.1440677969</v>
       </c>
-      <c r="H121" s="7"/>
-      <c r="I121" s="7"/>
-      <c r="J121" s="7"/>
-      <c r="K121" s="7">
+      <c r="H122" s="7"/>
+      <c r="I122" s="7"/>
+      <c r="J122" s="7"/>
+      <c r="K122" s="7">
         <f>SUM(K2:K119)</f>
         <v>118038800</v>
       </c>
-      <c r="L121" s="7">
+      <c r="L122" s="7">
         <f>SUM(L2:L120)</f>
         <v>16578502169009</v>
       </c>
-      <c r="M121" s="4">
+      <c r="M122" s="4">
         <f>SUM(M2:M120)</f>
         <v>3365919895100</v>
       </c>
-      <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-      <c r="Q121" s="4"/>
-      <c r="R121" s="4"/>
-      <c r="S121" s="4"/>
-      <c r="T121" s="4"/>
-      <c r="U121" s="4"/>
-      <c r="W121" s="4"/>
-      <c r="Y121" s="4"/>
-      <c r="Z121" s="4"/>
-      <c r="AA121" s="4"/>
-      <c r="AB121" s="4"/>
-      <c r="AC121" s="4"/>
-      <c r="AD121" s="4"/>
-      <c r="AE121" s="4"/>
-      <c r="AF121" s="4"/>
-      <c r="AG121" s="4"/>
-      <c r="AH121" s="4"/>
-      <c r="AI121" s="4"/>
-      <c r="AJ121" s="4"/>
-      <c r="AK121" s="4"/>
-      <c r="AL121" s="4"/>
-      <c r="AM121" s="4"/>
-      <c r="AN121" s="4"/>
-      <c r="AO121" s="4"/>
-      <c r="AP121" s="4"/>
-      <c r="AQ121" s="4"/>
-      <c r="AR121" s="4"/>
-      <c r="AY121" s="4"/>
-      <c r="AZ121" s="4"/>
-      <c r="BA121" s="4"/>
-      <c r="BB121" s="4"/>
-      <c r="BC121" s="4"/>
-      <c r="BD121" s="4"/>
-      <c r="BE121" s="3"/>
-      <c r="BF121" s="3"/>
-      <c r="BG121" s="3"/>
-      <c r="BH121" s="3"/>
-      <c r="BI121" t="e">
-        <f>#REF!-N121</f>
+      <c r="N122" s="4"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="4"/>
+      <c r="R122" s="4"/>
+      <c r="S122" s="4"/>
+      <c r="T122" s="4"/>
+      <c r="U122" s="4"/>
+      <c r="W122" s="4"/>
+      <c r="Y122" s="4"/>
+      <c r="Z122" s="4"/>
+      <c r="AA122" s="4"/>
+      <c r="AB122" s="4"/>
+      <c r="AC122" s="4"/>
+      <c r="AD122" s="4"/>
+      <c r="AE122" s="4"/>
+      <c r="AF122" s="4"/>
+      <c r="AG122" s="4"/>
+      <c r="AH122" s="4"/>
+      <c r="AI122" s="4"/>
+      <c r="AJ122" s="4"/>
+      <c r="AK122" s="4"/>
+      <c r="AL122" s="4"/>
+      <c r="AM122" s="4"/>
+      <c r="AN122" s="4"/>
+      <c r="AO122" s="4"/>
+      <c r="AP122" s="4"/>
+      <c r="AQ122" s="4"/>
+      <c r="AR122" s="4"/>
+      <c r="AY122" s="4"/>
+      <c r="AZ122" s="4"/>
+      <c r="BA122" s="4"/>
+      <c r="BB122" s="4"/>
+      <c r="BC122" s="4"/>
+      <c r="BD122" s="4"/>
+      <c r="BE122" s="3"/>
+      <c r="BF122" s="3"/>
+      <c r="BG122" s="3"/>
+      <c r="BH122" s="3"/>
+      <c r="BI122" t="e">
+        <f>#REF!-N122</f>
         <v>#REF!</v>
       </c>
-      <c r="BJ121" t="e">
+      <c r="BJ122" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="122" spans="1:62" ht="18">
-      <c r="D122" s="19"/>
-      <c r="Z122" s="12"/>
-      <c r="AB122" s="12"/>
-      <c r="AS122" s="12"/>
-      <c r="AW122" s="29"/>
     </row>
     <row r="123" spans="1:62" ht="18">
       <c r="D123" s="19"/>
       <c r="Z123" s="12"/>
-      <c r="AS123" s="19"/>
+      <c r="AB123" s="12"/>
+      <c r="AS123" s="12"/>
       <c r="AW123" s="29"/>
-      <c r="AY123">
+    </row>
+    <row r="124" spans="1:62" ht="18">
+      <c r="D124" s="19"/>
+      <c r="Z124" s="12"/>
+      <c r="AS124" s="19"/>
+      <c r="AW124" s="29"/>
+      <c r="AY124">
         <f>AY51-AY50</f>
         <v>35000</v>
       </c>
     </row>
-    <row r="124" spans="1:62" ht="18">
-      <c r="Z124" s="12"/>
-      <c r="AS124" s="19">
+    <row r="125" spans="1:62" ht="18">
+      <c r="Z125" s="12"/>
+      <c r="AS125" s="19">
         <v>10290000</v>
       </c>
-      <c r="AW124" s="29"/>
-      <c r="BB124">
+      <c r="AW125" s="29"/>
+      <c r="BB125">
         <f>AY60-AY59</f>
         <v>70000</v>
       </c>
     </row>
-    <row r="125" spans="1:62" ht="18">
-      <c r="G125">
-        <f>(G110-G121)/G121</f>
+    <row r="126" spans="1:62" ht="18">
+      <c r="G126">
+        <f>(G110-G122)/G122</f>
         <v>0.62241474570412092</v>
       </c>
-      <c r="V125" s="12"/>
-      <c r="Z125" s="12"/>
-      <c r="AS125" s="19"/>
-      <c r="AU125">
-        <f>AS124-AS49</f>
+      <c r="V126" s="12"/>
+      <c r="Z126" s="12"/>
+      <c r="AS126" s="19"/>
+      <c r="AU126">
+        <f>AS125-AS49</f>
         <v>195000</v>
       </c>
-      <c r="AW125" s="29">
+      <c r="AW126" s="29">
         <f>AC52-AY51</f>
         <v>305000</v>
       </c>
     </row>
-    <row r="126" spans="1:62" ht="18">
-      <c r="V126" s="12"/>
-      <c r="Z126" s="12"/>
-      <c r="AW126" s="29"/>
-    </row>
-    <row r="127" spans="1:62" ht="17.25" customHeight="1">
-      <c r="F127">
+    <row r="127" spans="1:62" ht="18">
+      <c r="V127" s="12"/>
+      <c r="Z127" s="12"/>
+      <c r="AW127" s="29"/>
+    </row>
+    <row r="128" spans="1:62" ht="17.25" customHeight="1">
+      <c r="F128">
         <f>(D112-F111)/F111</f>
         <v>3.7955768081291093E-2</v>
       </c>
-      <c r="V127" s="12"/>
-      <c r="Z127" s="12"/>
-    </row>
-    <row r="128" spans="1:62" ht="18">
-      <c r="D128">
+      <c r="V128" s="12"/>
+      <c r="Z128" s="12"/>
+    </row>
+    <row r="129" spans="4:49" ht="18">
+      <c r="D129">
         <f>(D112-F111)/F111</f>
         <v>3.7955768081291093E-2</v>
       </c>
-      <c r="V128" s="12"/>
-      <c r="Z128" s="12"/>
-      <c r="AW128">
-        <f>AW125/AY51</f>
+      <c r="V129" s="12"/>
+      <c r="Z129" s="12"/>
+      <c r="AW129">
+        <f>AW126/AY51</f>
         <v>2.9539951573849879E-2</v>
       </c>
     </row>
-    <row r="129" spans="22:22" ht="18">
-      <c r="V129" s="12"/>
-    </row>
-    <row r="130" spans="22:22" ht="18">
+    <row r="130" spans="4:49" ht="18">
       <c r="V130" s="12"/>
     </row>
+    <row r="131" spans="4:49" ht="18">
+      <c r="V131" s="12"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:BL125"/>
+  <autoFilter ref="A1:BL126"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -48585,10 +48796,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K689"/>
+  <dimension ref="A1:K700"/>
   <sheetViews>
-    <sheetView topLeftCell="A676" workbookViewId="0">
-      <selection activeCell="D693" sqref="D693"/>
+    <sheetView topLeftCell="A679" workbookViewId="0">
+      <selection activeCell="C691" sqref="C691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56352,8 +56563,178 @@
         <v>12140000</v>
       </c>
     </row>
+    <row r="692" spans="1:4">
+      <c r="A692" s="72" t="s">
+        <v>322</v>
+      </c>
+      <c r="B692" s="72"/>
+      <c r="C692" s="72"/>
+      <c r="D692" s="72"/>
+    </row>
+    <row r="693" spans="1:4">
+      <c r="A693" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B693" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C693" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D693" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="694" spans="1:4">
+      <c r="A694" s="43">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B694" s="3">
+        <v>27570</v>
+      </c>
+      <c r="C694" s="3">
+        <v>7530</v>
+      </c>
+      <c r="D694">
+        <v>12190000</v>
+      </c>
+    </row>
+    <row r="695" spans="1:4">
+      <c r="A695" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B695" s="3">
+        <v>27510</v>
+      </c>
+      <c r="C695" s="3">
+        <v>7530</v>
+      </c>
+      <c r="D695">
+        <v>12160000</v>
+      </c>
+    </row>
+    <row r="696" spans="1:4">
+      <c r="A696" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="B696" s="3">
+        <v>27560</v>
+      </c>
+      <c r="C696" s="3">
+        <v>7540</v>
+      </c>
+      <c r="D696">
+        <v>12190000</v>
+      </c>
+    </row>
+    <row r="697" spans="1:4">
+      <c r="A697" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B697" s="3">
+        <v>27530</v>
+      </c>
+      <c r="C697" s="3">
+        <v>7545</v>
+      </c>
+      <c r="D697">
+        <v>12180000</v>
+      </c>
+    </row>
+    <row r="698" spans="1:4">
+      <c r="A698" s="43">
+        <v>0.625</v>
+      </c>
+      <c r="B698" s="3">
+        <v>27530</v>
+      </c>
+      <c r="C698" s="3">
+        <v>7550</v>
+      </c>
+      <c r="D698">
+        <v>12190000</v>
+      </c>
+    </row>
+    <row r="699" spans="1:4">
+      <c r="A699" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B699" s="3">
+        <v>27530</v>
+      </c>
+      <c r="C699" s="3">
+        <v>7570</v>
+      </c>
+      <c r="D699">
+        <v>12210000</v>
+      </c>
+    </row>
+    <row r="700" spans="1:4">
+      <c r="A700" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="B700" s="3">
+        <v>27530</v>
+      </c>
+      <c r="C700" s="3">
+        <v>7570</v>
+      </c>
+      <c r="D700">
+        <v>12200000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="66">
+    <mergeCell ref="A692:D692"/>
+    <mergeCell ref="A658:D658"/>
+    <mergeCell ref="A647:D647"/>
+    <mergeCell ref="A635:D635"/>
+    <mergeCell ref="A623:D623"/>
+    <mergeCell ref="A612:D612"/>
+    <mergeCell ref="A555:D555"/>
+    <mergeCell ref="A544:D544"/>
+    <mergeCell ref="A511:D511"/>
+    <mergeCell ref="A467:D467"/>
+    <mergeCell ref="A500:D500"/>
+    <mergeCell ref="A489:D489"/>
+    <mergeCell ref="A478:D478"/>
+    <mergeCell ref="A522:D522"/>
+    <mergeCell ref="A243:D243"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A153:D153"/>
+    <mergeCell ref="A213:D213"/>
+    <mergeCell ref="A233:D233"/>
+    <mergeCell ref="A223:D223"/>
+    <mergeCell ref="A183:D183"/>
+    <mergeCell ref="A163:D163"/>
+    <mergeCell ref="A193:D193"/>
+    <mergeCell ref="A203:D203"/>
+    <mergeCell ref="A173:D173"/>
+    <mergeCell ref="A357:D357"/>
+    <mergeCell ref="A273:D273"/>
+    <mergeCell ref="A263:D263"/>
+    <mergeCell ref="A253:D253"/>
+    <mergeCell ref="A379:D379"/>
+    <mergeCell ref="A368:D368"/>
+    <mergeCell ref="A401:D401"/>
+    <mergeCell ref="A390:D390"/>
+    <mergeCell ref="A434:D434"/>
+    <mergeCell ref="A423:D423"/>
+    <mergeCell ref="A412:D412"/>
     <mergeCell ref="A681:D681"/>
     <mergeCell ref="A670:D670"/>
     <mergeCell ref="A283:D283"/>
@@ -56370,55 +56751,6 @@
     <mergeCell ref="A303:D303"/>
     <mergeCell ref="A445:D445"/>
     <mergeCell ref="A533:D533"/>
-    <mergeCell ref="A401:D401"/>
-    <mergeCell ref="A390:D390"/>
-    <mergeCell ref="A434:D434"/>
-    <mergeCell ref="A423:D423"/>
-    <mergeCell ref="A412:D412"/>
-    <mergeCell ref="A357:D357"/>
-    <mergeCell ref="A273:D273"/>
-    <mergeCell ref="A263:D263"/>
-    <mergeCell ref="A253:D253"/>
-    <mergeCell ref="A379:D379"/>
-    <mergeCell ref="A368:D368"/>
-    <mergeCell ref="A153:D153"/>
-    <mergeCell ref="A213:D213"/>
-    <mergeCell ref="A233:D233"/>
-    <mergeCell ref="A223:D223"/>
-    <mergeCell ref="A183:D183"/>
-    <mergeCell ref="A163:D163"/>
-    <mergeCell ref="A193:D193"/>
-    <mergeCell ref="A203:D203"/>
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="A243:D243"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A555:D555"/>
-    <mergeCell ref="A544:D544"/>
-    <mergeCell ref="A511:D511"/>
-    <mergeCell ref="A467:D467"/>
-    <mergeCell ref="A500:D500"/>
-    <mergeCell ref="A489:D489"/>
-    <mergeCell ref="A478:D478"/>
-    <mergeCell ref="A522:D522"/>
-    <mergeCell ref="A658:D658"/>
-    <mergeCell ref="A647:D647"/>
-    <mergeCell ref="A635:D635"/>
-    <mergeCell ref="A623:D623"/>
-    <mergeCell ref="A612:D612"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -56427,10 +56759,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M64"/>
+  <dimension ref="B1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M65" sqref="M65"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56494,7 +56826,7 @@
         <v>1060293</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:H64" si="0">(C3-C2)*100/C2</f>
+        <f t="shared" ref="F3:H65" si="0">(C3-C2)*100/C2</f>
         <v>-1.5820149875104079</v>
       </c>
       <c r="G3">
@@ -56523,7 +56855,7 @@
         <v>1074144</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F64" si="1">(C4-C3)*100/C3</f>
+        <f t="shared" ref="F4:F65" si="1">(C4-C3)*100/C3</f>
         <v>1.3959390862944163</v>
       </c>
       <c r="G4">
@@ -57808,7 +58140,7 @@
         <v>1.44</v>
       </c>
     </row>
-    <row r="49" spans="2:13">
+    <row r="49" spans="2:9">
       <c r="B49">
         <v>14000520</v>
       </c>
@@ -57837,7 +58169,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="50" spans="2:13">
+    <row r="50" spans="2:9">
       <c r="B50">
         <v>14000523</v>
       </c>
@@ -57866,7 +58198,7 @@
         <v>-0.26</v>
       </c>
     </row>
-    <row r="51" spans="2:13">
+    <row r="51" spans="2:9">
       <c r="B51">
         <v>14000524</v>
       </c>
@@ -57895,7 +58227,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="52" spans="2:13">
+    <row r="52" spans="2:9">
       <c r="B52">
         <v>14000531</v>
       </c>
@@ -57924,7 +58256,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="53" spans="2:13">
+    <row r="53" spans="2:9">
       <c r="B53">
         <v>14000601</v>
       </c>
@@ -57953,7 +58285,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="54" spans="2:13">
+    <row r="54" spans="2:9">
       <c r="B54">
         <v>14000602</v>
       </c>
@@ -57982,7 +58314,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="55" spans="2:13">
+    <row r="55" spans="2:9">
       <c r="B55">
         <v>14000603</v>
       </c>
@@ -58011,7 +58343,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="56" spans="2:13">
+    <row r="56" spans="2:9">
       <c r="B56">
         <v>14000606</v>
       </c>
@@ -58040,7 +58372,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="57" spans="2:13">
+    <row r="57" spans="2:9">
       <c r="B57">
         <v>14000607</v>
       </c>
@@ -58069,7 +58401,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="58" spans="2:13">
+    <row r="58" spans="2:9">
       <c r="B58">
         <v>14000608</v>
       </c>
@@ -58098,7 +58430,7 @@
         <v>-3.14</v>
       </c>
     </row>
-    <row r="59" spans="2:13">
+    <row r="59" spans="2:9">
       <c r="B59">
         <v>14000609</v>
       </c>
@@ -58127,7 +58459,7 @@
         <v>-1.82</v>
       </c>
     </row>
-    <row r="60" spans="2:13">
+    <row r="60" spans="2:9">
       <c r="B60">
         <v>14000610</v>
       </c>
@@ -58156,7 +58488,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="61" spans="2:13">
+    <row r="61" spans="2:9">
       <c r="B61">
         <v>14000613</v>
       </c>
@@ -58185,7 +58517,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="62" spans="2:13">
+    <row r="62" spans="2:9">
       <c r="B62">
         <v>14000614</v>
       </c>
@@ -58214,7 +58546,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="63" spans="2:13">
+    <row r="63" spans="2:9">
       <c r="B63">
         <v>14000615</v>
       </c>
@@ -58243,7 +58575,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="64" spans="2:13">
+    <row r="64" spans="2:9">
       <c r="B64">
         <v>14000616</v>
       </c>
@@ -58271,17 +58603,46 @@
       <c r="I64">
         <v>-1</v>
       </c>
-      <c r="J64">
-        <v>0.41</v>
-      </c>
-      <c r="K64">
-        <v>0.75</v>
-      </c>
-      <c r="L64">
-        <v>0.73</v>
-      </c>
-      <c r="M64">
-        <v>-1</v>
+    </row>
+    <row r="65" spans="2:13">
+      <c r="B65">
+        <v>14000617</v>
+      </c>
+      <c r="C65" s="54">
+        <v>27530</v>
+      </c>
+      <c r="D65">
+        <v>12200000</v>
+      </c>
+      <c r="E65">
+        <v>1174333</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>1.5117994100294985</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>0.49423393739703458</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="0"/>
+        <v>9.8365211105892622E-2</v>
+      </c>
+      <c r="I65">
+        <v>0.19</v>
+      </c>
+      <c r="J65">
+        <v>1.51</v>
+      </c>
+      <c r="K65">
+        <v>0.49</v>
+      </c>
+      <c r="L65">
+        <v>0.1</v>
+      </c>
+      <c r="M65">
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>